<commit_message>
Home, Register, Login and LinkedList modules added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/DsAlgo_TestData.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4C76A9B0-5713-4570-B959-580C5C70B1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rinuh\eclipse-workspace\TestNG_Latest\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A4CE07-EEA0-41E4-9EB4-78D1B61D74BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Valid" sheetId="1" r:id="rId1"/>
@@ -14,8 +19,7 @@
     <sheet name="TryEditor" sheetId="4" r:id="rId4"/>
     <sheet name="Array" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A1:N32"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,13 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
   <si>
     <t>Codecrackers</t>
   </si>
@@ -60,15 +58,6 @@
     <t>Admin@1234</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>PasswordConfirmation</t>
-  </si>
-  <si>
     <t>adminninja</t>
   </si>
   <si>
@@ -103,9 +92,6 @@
   </si>
   <si>
     <t>code@123</t>
-  </si>
-  <si>
-    <t>Admin1@567</t>
   </si>
   <si>
     <t>pythoncode</t>
@@ -263,12 +249,48 @@
   <si>
     <t>[4, 9, 9, 49, 121]</t>
   </si>
+  <si>
+    <t>You are logged in</t>
+  </si>
+  <si>
+    <t>Logged out successfully</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>Invalid Username and Password</t>
+  </si>
+  <si>
+    <t>MESSAGE</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>PASSWORD CONFIRMATION</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>New Account Created. You are logged in as</t>
+  </si>
+  <si>
+    <t>code$^&amp;()_+)(*</t>
+  </si>
+  <si>
+    <t>Sample@9093</t>
+  </si>
+  <si>
+    <t>SampleTest@3237</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,30 +310,6 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Display"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -336,16 +334,35 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -383,6 +400,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -390,40 +433,42 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -686,35 +731,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19" style="10" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.77734375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="3" spans="1:3" ht="31.8" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
@@ -725,67 +775,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.21875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.21875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C4" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{2F3F871B-2916-4F86-A469-A19A299FA857}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{DE1B72FB-F396-4B0F-801E-B4BFF38C3894}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -794,172 +878,262 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="15.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.21875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="50.44140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="12" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="13">
+        <v>12345678</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="13"/>
+      <c r="B6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="13"/>
+      <c r="B7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="13"/>
+      <c r="B8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="13"/>
+      <c r="B9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="B11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="11">
         <v>12345678</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
+      <c r="C13" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="72" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+      <c r="C14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="13"/>
+      <c r="B15" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="8">
-        <v>12345678</v>
-      </c>
-      <c r="C13" s="8">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>25</v>
+      <c r="C15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" display="mailto:Admin@123" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C10" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="C11" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
     <hyperlink ref="B15" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
     <hyperlink ref="C15" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
     <hyperlink ref="C16" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
@@ -967,6 +1141,7 @@
     <hyperlink ref="A18" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
     <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
     <hyperlink ref="C18" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{BDF4048E-1A9E-471B-AA76-0B91A494AA63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -977,7 +1152,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -987,34 +1164,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1040,324 +1217,324 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+    </row>
+    <row r="2" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:27" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:27" ht="177" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="11" t="s">
+    </row>
+    <row r="5" spans="1:27" ht="177" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-    </row>
-    <row r="2" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="B5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="14"/>
-    </row>
-    <row r="3" spans="1:27" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:27" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="14"/>
-    </row>
-    <row r="4" spans="1:27" ht="177" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:27" ht="252" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:27" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:27" ht="192.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" ht="177" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="B9" s="6">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:27" ht="193.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:27" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="15"/>
-    </row>
-    <row r="6" spans="1:27" ht="147" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="B11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="1:27" ht="252" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-    </row>
-    <row r="8" spans="1:27" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:27" ht="192.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="14">
-        <v>2</v>
-      </c>
-      <c r="C9" s="14"/>
-    </row>
-    <row r="10" spans="1:27" ht="193.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:27" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="14"/>
-    </row>
-    <row r="11" spans="1:27" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="14"/>
-    </row>
-    <row r="12" spans="1:27" ht="147" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
     </row>
     <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
     </row>
     <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>